<commit_message>
PrePlacement training notes and Java & Python roadmap are included
</commit_message>
<xml_diff>
--- a/1 Training Plans/1 Pre_Placement_Plan_Dream_Track.xlsx
+++ b/1 Training Plans/1 Pre_Placement_Plan_Dream_Track.xlsx
@@ -13,6 +13,8 @@
     <sheet name="Domain Specific - Data Analysis" sheetId="6" r:id="rId10"/>
     <sheet name="Domain Specific - Machine Learn" sheetId="7" r:id="rId11"/>
     <sheet name="Problem Solving RoadMap" sheetId="8" r:id="rId12"/>
+    <sheet name="Java RoadMap - Java RoadMap" sheetId="9" r:id="rId13"/>
+    <sheet name="Python RoadMap - Python RoadMap" sheetId="10" r:id="rId14"/>
   </sheets>
 </workbook>
 </file>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="871">
   <si>
     <t>3RD YR PRE PLACEMENT TRAINING</t>
   </si>
@@ -3332,6 +3334,2396 @@
   </si>
   <si>
     <t>Great for mock interviews.</t>
+  </si>
+  <si>
+    <t>Java RoadMap</t>
+  </si>
+  <si>
+    <t>Topics to Learn</t>
+  </si>
+  <si>
+    <t>Practice Problems (Updated &amp; Extended)</t>
+  </si>
+  <si>
+    <t>LeetCode Problems</t>
+  </si>
+  <si>
+    <t>Phase 1: Java Basics + Aptitude Warmup</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Java Setup (JDK, IDE) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Variables &amp; Data Types 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Input/Output (Scanner) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Operators 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Conditionals (if-else, switch) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Loops (for, while, do-while)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Math/Aptitude Easy:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Simple &amp; Compound Interest 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Area &amp; Perimeter (Circle, Rectangle, Triangle)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Celsius ↔ Fahrenheit conversion
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Largest of 3 numbers
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Leap Year Checker
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Power of number (a^b) without Math.pow
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">GCD &amp; LCM (loops) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Coding Easy:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Even/Odd
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Swap numbers (with/without temp)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Sum of first N numbers
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Multiplication table
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Simple Calculator (switch)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Prime Check
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Print divisors of a number 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Patterns:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Star/Number Pyramid
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Floyd’s Triangle</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">1523. Count Odd Numbers in Interval Range
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">1480. Running Sum of Array
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>1342. Number of Steps to Reduce to Zero</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase 2: Arrays + Strings + Math</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Arrays (1D, 2D)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Strings (basics) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Methods (functions, return types) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Recursion basics</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Math/Aptitude Medium:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">HCF/LCM (efficient)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Reverse digits / Armstrong number
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Digit sum &amp; digit product
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Quadratic equation solver 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Coding Medium (Arrays + Strings):
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Reverse an array
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Find min &amp; max
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">2nd largest element (no sort)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Move zeros to end
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Merge two sorted arrays
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Kadane’s Algorithm: Max Subarray Sum
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Frequency counter (HashMap)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Count vowels in string
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Remove duplicate characters
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Palindrome (string/number)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Anagram Check 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Recursion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Fibonacci (loop &amp; recursion)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Factorial
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Sum of digits</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">1. Two Sum
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">9. Palindrome Number
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">13. Roman to Integer
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">217. Contains Duplicate
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>344. Reverse String</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase 3: OOPs Concepts</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Classes &amp; Objects
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Constructors
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Inheritance
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Polymorphism (overload/override)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Abstraction &amp; Interfaces
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Encapsulation (getters/setters)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Application Medium:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Bank Account System (deposit/withdraw/balance)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Student class (avg marks, grade calc)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Shape hierarchy (circle, rectangle → area)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Employee hierarchy (Manager, Developer)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Library System (book → author mapping) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Additional OOP Tasks:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Calculator using Interface (add/sub/mul/div)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Vehicle → Car/Bike (override mileage)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Payment system (UPI/Card/Wallet polymorphism)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">College → Department → Student aggregation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Export Student Report to .txt (File + OOP)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">707. Design Linked List
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">225. Implement Stack using Queues
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>232. Implement Queue using Stacks</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase 4: DSA with Java</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Collections (ArrayList, HashMap, HashSet, LinkedList, Stack, Queue, PriorityQueue)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Comparator
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Sorting (Bubble, Selection, Insertion, Merge, Quick)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Searching (Linear, Binary)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Problem Solving Hard:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Implement Stack &amp; Queue manually
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">HashMap frequency counter
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Find duplicates in array
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Sorting student marks
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Matrix operations (transpose/diagonal sum) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>DSA Must-Do Algorithms:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Merge Sort
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Quick Sort
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Counting Sort (basic)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Two Pointer Pair Sum
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Reverse LinkedList (iter + rec)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Detect/Remove Cycle in LL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Sliding Window Max (Deque)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Spiral + Rotate Matrix (90°)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Infix → Postfix → Evaluation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">20. Valid Parentheses
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">242. Valid Anagram
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">49. Group Anagrams
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">347. Top K Frequent Elements
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>56. Merge Intervals</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase 5: Real-World Java</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">File Handling (read/write)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Exception Handling
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Streams &amp; Lambdas
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>JDBC basics</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Application Hard:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">ATM Simulation (PIN, withdraw, balance log)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Student Management System (CRUD)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Online Shopping Cart
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">File-based word frequency counter
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Library Management Mini-System 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Additional Real-Time Projects:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Railway Ticket Reservation System
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Hospital Appointment Booking
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Expense Tracker App (CSV/PDF report)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">To-Do Task Scheduler
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Quiz Application (MCQ scoring)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">146. LRU Cache
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">295. Median from Data Stream
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>380. Insert Delete GetRandom O(1)</t>
+    </r>
+  </si>
+  <si>
+    <t>Python RoadMap</t>
+  </si>
+  <si>
+    <t>Practice Problems (Core + Must Solve)</t>
+  </si>
+  <si>
+    <t>Phase 1: Python Basics + Aptitude Warmup</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Installation (Python, VS Code, IDEs)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Variables &amp; Data Types
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Input/Output
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Operators
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Conditionals (if-elif-else)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Loops (for, while)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Type Casting
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Basic Math &amp; String functions</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Math/Aptitude Easy: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Simple &amp; Compound Interest 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Unit conversions (temp, km↔miles)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Area/Perimeter of shapes
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Max of 3 numbers 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Leap year checker 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Decimal → Binary conversion 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Coding Basics: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Even/Odd
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Swap two numbers
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Sum of N natural numbers
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Multiplication table
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Factorial (loop) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Patterns: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Stars / number pyramids 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Floyd’s triangle</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">1480. Running Sum of Array
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">1523. Count Odd Numbers in Interval
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>1342. Reduce Number to Zero</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase 2: Lists, Tuples, Strings, Functions</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Lists, Tuples, Sets, Dict
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">List methods &amp; slicing
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Functions + params + return
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Lambda, map, filter, reduce
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Recursion basics
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>String operations</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">List &amp; String Drills: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Reverse list/string 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Find max/min in list 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Second largest without sort 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Merge two sorted lists 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Move zeros to end 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Count vowels in string 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Character frequency dict 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Remove duplicates from string 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Check Palindrome 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Check Anagram 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Recursion: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Fibonacci (rec)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Factorial (rec)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Sum of digits</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">1. Two Sum
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">9. Palindrome Number
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">217. Contains Duplicate
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">344. Reverse String
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>13. Roman to Integer</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase 3: Core Python + File / Exception Handling</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">File Handling (read/write)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Exception Handling (try/except)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Modules &amp; Packages
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Comprehensions (List/Dict/Set Gen)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Iterators &amp; Generators
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Virtual env &amp; pip basics</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Hands-On Projects: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Word counter tool
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">File case converter (upper/lower/title)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Student grade calculator storing output in file
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">JSON save-load notes app 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Object Based: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Library File Export (.txt/.json)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Log writer with error handling</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">20. Valid Parentheses (stack logic)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">49. Group Anagrams (dict/hashmap)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>242. Valid Anagram</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase 4: Python OOP + DSA (Placement Zone)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Classes &amp; Objects
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">OOP Pillars (Encap, Inheritance, Poly, Abstraction)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">DSA Using Python Lists/Dict
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Time Complexity (Big-O)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Searching (Linear/Binary)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Sorting (Bubble, Selection, Insertion, Merge, Quick)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Linked Lists, Stacks, Queues, Trees, Graphs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Core DSA Must-Solve: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Implement Stack &amp; Queue (list/deque) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Linked List insert/delete/reverse
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Detect cycle in linked list
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Two Sum using HashMap
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Sliding Window max
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Top K frequent elements
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Binary Search problems
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Spiral traversal of matrix
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Rotate matrix 90°
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Merge intervals</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">21. Merge Two Sorted Lists
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">206. Reverse Linked List
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">141. Linked List Cycle
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">347. Top K Frequent Elements
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>56. Merge Intervals</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase 5: Advanced Python + Real-Time Integration</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Modules: os, sys, datetime, collections
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Regular Expressions (re)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Decorators
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Itertools &amp; Functools
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">SQLite/MySQL with Python DB API
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Multi-threading &amp; Multiprocessing
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>APIs (requests)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Mini Projects (Real World): 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Password Generator with strength meter 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">To-Do CLI app (file/json store) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Expense Tracker + CSV reports
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">URL Shortener
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Blog CRUD using SQLite
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Weather API fetcher
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>PDF Invoice Creator</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase 6 (Optional but Powerful): Python for Automation + Web + ML</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Selenium Web Automation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">FastAPI/Flask REST backend
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Data Analysis (Pandas/Numpy)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Visualization (Matplotlib/Plotly)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>ML Introduction (Sklearn)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Build-Level Projects:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Auto-mail sender tool 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Web Scraper (news/jobs)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Flask Login+Register System
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Student Result Dashboard (CSV → Graph)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Face Recognition Attendance</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">53. Max Subarray (Kadane)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">347. Top K Frequent Elements
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>238. Product of Array Except Self</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3343,7 +5735,7 @@
     <numFmt numFmtId="59" formatCode="ddd, d mmm yyyy"/>
     <numFmt numFmtId="60" formatCode="dddd, d mmmm yyyy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -3417,6 +5809,18 @@
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="16"/>
+      <color indexed="25"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -3468,7 +5872,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -3655,13 +6059,118 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="26"/>
+      </left>
+      <right style="thin">
+        <color indexed="26"/>
+      </right>
+      <top style="thin">
+        <color indexed="26"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="27"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="26"/>
+      </left>
+      <right style="thin">
+        <color indexed="27"/>
+      </right>
+      <top style="thin">
+        <color indexed="27"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="26"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="27"/>
+      </left>
+      <right style="thin">
+        <color indexed="26"/>
+      </right>
+      <top style="thin">
+        <color indexed="27"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="26"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="26"/>
+      </left>
+      <right style="thin">
+        <color indexed="26"/>
+      </right>
+      <top style="thin">
+        <color indexed="27"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="26"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="26"/>
+      </left>
+      <right style="thin">
+        <color indexed="27"/>
+      </right>
+      <top style="thin">
+        <color indexed="26"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="26"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="27"/>
+      </left>
+      <right style="thin">
+        <color indexed="26"/>
+      </right>
+      <top style="thin">
+        <color indexed="26"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="26"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="26"/>
+      </left>
+      <right style="thin">
+        <color indexed="26"/>
+      </right>
+      <top style="thin">
+        <color indexed="26"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="26"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3941,6 +6450,51 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="1" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="1" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="1" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="1" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4063,6 +6617,9 @@
       <rgbColor rgb="ffffd38a"/>
       <rgbColor rgb="ffff9781"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffed220b"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -5392,6 +7949,144 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="16.3516" style="104" customWidth="1"/>
+    <col min="2" max="2" width="48.4844" style="104" customWidth="1"/>
+    <col min="3" max="3" width="48.6719" style="104" customWidth="1"/>
+    <col min="4" max="4" width="38.1172" style="104" customWidth="1"/>
+    <col min="5" max="16384" width="16.3516" style="104" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="26.5" customHeight="1">
+      <c r="A1" t="s" s="94">
+        <v>846</v>
+      </c>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+    </row>
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" t="s" s="95">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="95">
+        <v>823</v>
+      </c>
+      <c r="C2" t="s" s="95">
+        <v>847</v>
+      </c>
+      <c r="D2" t="s" s="95">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="3" ht="239.9" customHeight="1">
+      <c r="A3" t="s" s="96">
+        <v>848</v>
+      </c>
+      <c r="B3" t="s" s="97">
+        <v>849</v>
+      </c>
+      <c r="C3" t="s" s="98">
+        <v>850</v>
+      </c>
+      <c r="D3" t="s" s="99">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="4" ht="224.7" customHeight="1">
+      <c r="A4" t="s" s="100">
+        <v>852</v>
+      </c>
+      <c r="B4" t="s" s="101">
+        <v>853</v>
+      </c>
+      <c r="C4" t="s" s="102">
+        <v>854</v>
+      </c>
+      <c r="D4" t="s" s="103">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="5" ht="119.7" customHeight="1">
+      <c r="A5" t="s" s="100">
+        <v>856</v>
+      </c>
+      <c r="B5" t="s" s="101">
+        <v>857</v>
+      </c>
+      <c r="C5" t="s" s="102">
+        <v>858</v>
+      </c>
+      <c r="D5" t="s" s="103">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="6" ht="164.7" customHeight="1">
+      <c r="A6" t="s" s="100">
+        <v>860</v>
+      </c>
+      <c r="B6" t="s" s="101">
+        <v>861</v>
+      </c>
+      <c r="C6" t="s" s="102">
+        <v>862</v>
+      </c>
+      <c r="D6" t="s" s="103">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="7" ht="119.7" customHeight="1">
+      <c r="A7" t="s" s="100">
+        <v>864</v>
+      </c>
+      <c r="B7" t="s" s="101">
+        <v>865</v>
+      </c>
+      <c r="C7" t="s" s="102">
+        <v>866</v>
+      </c>
+      <c r="D7" t="s" s="103">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="8" ht="95.7" customHeight="1">
+      <c r="A8" t="s" s="105">
+        <v>867</v>
+      </c>
+      <c r="B8" t="s" s="106">
+        <v>868</v>
+      </c>
+      <c r="C8" t="s" s="107">
+        <v>869</v>
+      </c>
+      <c r="D8" t="s" s="107">
+        <v>870</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:G183"/>
@@ -12208,4 +14903,128 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="16.3516" style="93" customWidth="1"/>
+    <col min="2" max="2" width="52.3125" style="93" customWidth="1"/>
+    <col min="3" max="3" width="57.2734" style="93" customWidth="1"/>
+    <col min="4" max="4" width="43.2344" style="93" customWidth="1"/>
+    <col min="5" max="16384" width="16.3516" style="93" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="26.5" customHeight="1">
+      <c r="A1" t="s" s="94">
+        <v>822</v>
+      </c>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+    </row>
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" t="s" s="95">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="95">
+        <v>823</v>
+      </c>
+      <c r="C2" t="s" s="95">
+        <v>824</v>
+      </c>
+      <c r="D2" t="s" s="95">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="3" ht="284.9" customHeight="1">
+      <c r="A3" t="s" s="96">
+        <v>826</v>
+      </c>
+      <c r="B3" t="s" s="97">
+        <v>827</v>
+      </c>
+      <c r="C3" t="s" s="98">
+        <v>828</v>
+      </c>
+      <c r="D3" t="s" s="99">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="4" ht="314.7" customHeight="1">
+      <c r="A4" t="s" s="100">
+        <v>830</v>
+      </c>
+      <c r="B4" t="s" s="101">
+        <v>831</v>
+      </c>
+      <c r="C4" t="s" s="102">
+        <v>832</v>
+      </c>
+      <c r="D4" t="s" s="103">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="5" ht="179.7" customHeight="1">
+      <c r="A5" t="s" s="100">
+        <v>834</v>
+      </c>
+      <c r="B5" t="s" s="101">
+        <v>835</v>
+      </c>
+      <c r="C5" t="s" s="102">
+        <v>836</v>
+      </c>
+      <c r="D5" t="s" s="103">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="6" ht="239.7" customHeight="1">
+      <c r="A6" t="s" s="100">
+        <v>838</v>
+      </c>
+      <c r="B6" t="s" s="101">
+        <v>839</v>
+      </c>
+      <c r="C6" t="s" s="102">
+        <v>840</v>
+      </c>
+      <c r="D6" t="s" s="103">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="7" ht="179.7" customHeight="1">
+      <c r="A7" t="s" s="100">
+        <v>842</v>
+      </c>
+      <c r="B7" t="s" s="101">
+        <v>843</v>
+      </c>
+      <c r="C7" t="s" s="102">
+        <v>844</v>
+      </c>
+      <c r="D7" t="s" s="103">
+        <v>845</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>